<commit_message>
agrega tabla y logo (gracias Vir)
</commit_message>
<xml_diff>
--- a/data/proyectos_ec.xlsx
+++ b/data/proyectos_ec.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="65">
   <si>
     <t>Finlandia</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Plan de acción en Economía Circular</t>
   </si>
 </sst>
 </file>
@@ -542,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1074,7 +1077,9 @@
       <c r="A48" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C48" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filtra por visión de economía circular
</commit_message>
<xml_diff>
--- a/data/proyectos_ec.xlsx
+++ b/data/proyectos_ec.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="65">
   <si>
     <t>Finlandia</t>
   </si>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1080,7 +1080,9 @@
       <c r="B48" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>